<commit_message>
fixed erronous RV in qualitative inspection data for chapter 4
</commit_message>
<xml_diff>
--- a/raw_data/highest_lowest_RV_for_inspection_data.xlsx
+++ b/raw_data/highest_lowest_RV_for_inspection_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peder\Dropbox\jobb\PhD\Projects\2019_NeuroRep_Replication_Value\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA4A5D34-2041-4CCC-B992-7D8422F510D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F91CF04-0A9D-4D20-92B6-2B734D03C76B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3600" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="highest_lowest_RV_for_inspectio" sheetId="1" r:id="rId1"/>
@@ -124,18 +124,6 @@
     <t>Perception of emotion is critical for successful social interaction, yet the neural mechanisms underlying the perception of dynamic, audio-visual emotional cues are poorly understood. Evidence from language and sensory paradigms suggests that the superior temporal sulcus and gyrus (STS/STG) play a key role in the integration of auditory and visual cues. Emotion perception research has focused on static facial cues; however, dynamic audio-visual (AV) cues mimic real-world social cues more accurately than static and/or unimodal stimuli. Novel dynamic AV stimuli were presented using a block design in two fMRI studies, comparing bimodal stimuli to unimodal conditions, and emotional to neutral stimuli. Results suggest that the bilateral superior temporal region plays distinct roles in the perception of emotion and in the integration of auditory and visual cues. Given the greater ecological validity of the stimuli developed for this study, this paradigm may be helpful in elucidating the deficits in emotion perception experienced by clinical populations. (C) 2008 Elsevier Inc. All rights reserved.</t>
   </si>
   <si>
-    <t>10.3389/fnhum.2018.00218</t>
-  </si>
-  <si>
-    <t>Cooperative and Competitive Contextual Effects on Social Cognitive and Empathic Neural Responses</t>
-  </si>
-  <si>
-    <t>Lee, M; Ahn, HS; Kwon, SK; Kim, SI</t>
-  </si>
-  <si>
-    <t>We aimed to differentiate the neural responses to cooperative and competitive contexts, which are the two of the most important social contexts in human society. Healthy male college students were asked to complete a Tetris-like task requiring mental rotation skills under individual, cooperative, and competitive contexts in an fMRI scanner. While the participants completed the task, pictures of others experiencing pain evoking emotional empathy randomly appeared to capture contextual effects on empathic neural responses. Behavioral results indicated that, in the presence of cooperation, participants solved the tasks more accurately and quickly than what they did when in the presence of competition. The fMRI results revealed activations in the dorsolateral prefrontal cortex (dIPFC) and dorsomedial prefrontal cortex (dmPFC) related to executive functions and theory of mind when participants performed the task under both cooperative and competitive contexts, whereas no activation of such areas was observed in the individual context. Cooperation condition exhibited stronger neural responses in the ventromedial prefrontal cortex (vmPFC) and dmPFC than competition condition. Competition condition, however, showed marginal neural responses in the cerebellum and anterior insular cortex (AIC). The two social contexts involved stronger empathic neural responses to other's pain than the individual context, but no substantial differences between cooperation and competition were present. Regions of interest analyses revealed that individual's trait empathy modulated the neural activity in the state empathy network, the AIC, and the dorsal anterior cingulate cortex (dACC) depending on the social context. These results suggest that cooperation improves task performance and activates neural responses associated with reward and mentalizing. Furthermore, the interaction between trait- and state-empathy was explored by correlation analyses between individual's trait empathy score and changing empathic brain activations along with the exposure to the cooperative and competitive social contexts.</t>
-  </si>
-  <si>
     <t>10.1016/j.neuroimage.2008.09.062</t>
   </si>
   <si>
@@ -160,18 +148,6 @@
     <t>We attempt to determine the discriminability and organization of neural activation corresponding to the experience of specific emotions. Method actors were asked to self-induce nine emotional states (anger, disgust, envy, fear, happiness, lust, pride, sadness, and shame) while in an fMRI scanner. Using a Gaussian Naive Bayes pooled variance classifier, we demonstrate the ability to identify specific emotions experienced by an individual at well over chance accuracy on the basis of: 1) neural activation of the same individual in other trials, 2) neural activation of other individuals who experienced similar trials, and 3) neural activation of the same individual to a qualitatively different type of emotion induction. Factor analysis identified valence, arousal, sociality, and lust as dimensions underlying the activation patterns. These results suggest a structure for neural representations of emotion and inform theories of emotional processing.</t>
   </si>
   <si>
-    <t>10.1093/cercor/bhw068</t>
-  </si>
-  <si>
-    <t>A Model of Representational Spaces in Human Cortex</t>
-  </si>
-  <si>
-    <t>Guntupalli, JS; Hanke, M; Halchenko, YO; Connolly, AC; Ramadge, PJ; Haxby, JV</t>
-  </si>
-  <si>
-    <t>Current models of the functional architecture of human cortex emphasize areas that capture coarse-scale features of cortical topography but provide no account for population responses that encode information in fine-scale patterns of activity. Here, we present a linear model of shared representational spaces in human cortex that captures fine-scale distinctions among population responses with response-tuning basis functions that are common across brains and models cortical patterns of neural responses with individual-specific topographic basis functions. We derive a common model space for the whole cortex using a new algorithm, searchlight hyperalignment, and complex, dynamic stimuli that provide a broad sampling of visual, auditory, and social percepts. The model aligns representations across brains in occipital, temporal, parietal, and prefrontal cortices, as shown by between-subject multivariate pattern classification and intersubject correlation of representational geometry, indicating that structural principles for shared neural representations apply across widely divergent domains of information. The model provides a rigorous account for individual variability of well-known coarse-scale topographies, such as retinotopy and category selectivity, and goes further to account for fine-scale patterns that are multiplexed with coarse-scale topographies and carry finer distinctions.</t>
-  </si>
-  <si>
     <t>10.1073/pnas.1202129109</t>
   </si>
   <si>
@@ -370,18 +346,6 @@
     <t>The purpose of this study was to assess functional changes in the cerebral cortex in people with different sign language experience and hearing status whilst observing and imitating Chinese Sign Language (CSL) using functional magnetic resonance imaging (fMRI). 50 participants took part in the study, and were divided into four groups according to their hearing status and experience of using sign language: prelingual deafness signer group (PDS), normal hearing non-signer group (HnS), native signer group with normal hearing (HNS), and acquired signer group with normal hearing (HLS). fMRI images were scanned from all subjects when they performed block-designed tasks that involved observing and imitating sign language stimuli. Nine activation areas were found in response to undertaking either observation or imitation CSL tasks and three activated areas were found only when undertaking the imitation task. Of those, the PDS group had significantly greater activation areas in terms of the cluster size of the activated voxels in the bilateral superior parietal lobule, cuneate lobe and lingual gyrus in response to undertaking either the observation or the imitation CSL task than the HnS, HNS and HLS groups. The PDS group also showed significantly greater activation in the bilateral inferior frontal gyrus which was also found in the HNS or the HLS groups but not in the HnS group. This indicates that deaf signers have better sign language proficiency, because they engage more actively with the phonetic and semantic elements. In addition, the activations of the bilateral superior temporal gyrus and inferior parietal lobule were only found in the PDS group and HNS group, and not in the other two groups, which indicates that the area for sign language processing appears to be sensitive to the age of language acquisition. Learning Outcomes: After reading this article, readers will be able to: discuss the relationship between sign language and its neural mechanisms. (C) 2014 Elsevier Inc. All rights reserved.</t>
   </si>
   <si>
-    <t>10.1097/WNR.0b013e32835ad307</t>
-  </si>
-  <si>
-    <t>A funny thing happened on the way to the scanner: humor detection correlates with gray matter volume</t>
-  </si>
-  <si>
-    <t>Kipman, M; Weber, M; Schwab, ZJ; DelDonno, SR; Killgore, WDS</t>
-  </si>
-  <si>
-    <t>The detection and appreciation of humor is a complex cognitive process that remains poorly understood. Although functional neuroimaging studies have begun to map the brain systems involved in humor appreciation, there are virtually no data on the structural correlates between gray matter volume and this capacity. Using voxel-based morphometry, the present study examined the association between gray matter volume and the ability to detect and appreciate humor. Fifty-nine healthy adults aged 18-45 years (30 men) underwent structural MRI and completed the University of Pennsylvania Humor Appreciation Test (HAT). After controlling for age and sex, gray matter volume of the left inferior frontal gyrus, left temporal pole, and left insula correlated positively with the appreciation of visual and verbal humor on the HAT, whereas the gray matter volume of the right inferior frontal gyrus correlated only with verbal humor appreciation scores. There were no negative correlations between gray matter volume and HAT performance. These data support a neurobiological basis for humor appreciation, particularly involving left-hemispheric cortical systems, and further suggest that individual differences in humor appreciation may be related to differences in regional gray matter volume. NeuroReport 23:1059-1064 (C) 2012 Wolters Kluwer Health \ Lippincott Williams &amp; Wilkins.</t>
-  </si>
-  <si>
     <t>10.1016/j.neuroscience.2017.06.003</t>
   </si>
   <si>
@@ -598,18 +562,12 @@
     <t>WOS:000263581900006</t>
   </si>
   <si>
-    <t>WOS:000434825200001</t>
-  </si>
-  <si>
     <t>WOS:000262301500012</t>
   </si>
   <si>
     <t>WOS:000322361200050</t>
   </si>
   <si>
-    <t>WOS:000377917500044</t>
-  </si>
-  <si>
     <t>WOS:000304445800031</t>
   </si>
   <si>
@@ -658,9 +616,6 @@
     <t>WOS:000341066700005</t>
   </si>
   <si>
-    <t>WOS:000311107800006</t>
-  </si>
-  <si>
     <t>WOS:000406984900018</t>
   </si>
   <si>
@@ -710,6 +665,51 @@
   </si>
   <si>
     <t>comments</t>
+  </si>
+  <si>
+    <t>WOS:000280503500019</t>
+  </si>
+  <si>
+    <t>10.1523/JNEUROSCI.2161-10.2010</t>
+  </si>
+  <si>
+    <t>Supramodal Representations of Perceived Emotions in the Human Brain</t>
+  </si>
+  <si>
+    <t>Peelen, MV; Atkinson, AP; Vuilleumier, P</t>
+  </si>
+  <si>
+    <t>Basic emotional states (such as anger, fear, and joy) can be similarly conveyed by the face, the body, and the voice. Are there human brain regions that represent these emotional mental states regardless of the sensory cues from which they are perceived? To address this question, in the present study participants evaluated the intensity of emotions perceived from face movements, body movements, or vocal intonations, while their brain activity was measured with functional magnetic resonance imaging (fMRI). Using multivoxel pattern analysis, we compared the similarity of response patterns across modalities to test for brain regions in which emotion-specific patterns in one modality (e. g., faces) could predict emotion-specific patterns in another modality (e. g., bodies). A whole-brain searchlight analysis revealed modality-independent but emotion category-specific activity patterns in medial prefrontal cortex (MPFC) and left superior temporal sulcus (STS). Multivoxel patterns in these regions contained information about the category of the perceived emotions (anger, disgust, fear, happiness, sadness) across all modality comparisons (face-body, face-voice, body-voice), and independently of the perceived intensity of the emotions. No systematic emotion-related differences were observed in the overall amplitude of activation in MPFC or STS. These results reveal supramodal representations of emotions in high-level brain areas previously implicated in affective processing, mental state attribution, and theory-of-mind. We suggest that MPFC and STS represent perceived emotions at an abstract, modality-independent level, and thus play a key role in the understanding and categorization of others' emotional mental states.</t>
+  </si>
+  <si>
+    <t>WOS:000263295400043</t>
+  </si>
+  <si>
+    <t>10.1126/science.1165604</t>
+  </si>
+  <si>
+    <t>When Your Gain Is My Pain and Your Pain Is My Gain: Neural Correlates of Envy and Schadenfreude</t>
+  </si>
+  <si>
+    <t>Takahashi, H; Kato, M; Matsuura, M; Mobbs, D; Suhara, T; Okubo, Y</t>
+  </si>
+  <si>
+    <t>We often evaluate the self and others from social comparisons. We feel envy when the target person has superior and self- relevant characteristics. Schadenfreude occurs when envied persons fall from grace. To elucidate the neurocognitive mechanisms of envy and schadenfreude, we conducted two functional magnetic resonance imaging studies. In study one, the participants read information concerning target persons characterized by levels of possession and self- relevance of comparison domains. When the target person's possession was superior and self- relevant, stronger envy and stronger anterior cingulate cortex ( ACC) activation were induced. In study two, stronger schadenfreude and stronger striatum activation were induced when misfortunes happened to envied persons. ACC activation in study one predicted ventral striatum activation in study two. Our findings document mechanisms of painful emotion, envy, and a rewarding reaction, schadenfreude.</t>
+  </si>
+  <si>
+    <t>WOS:000436471500009</t>
+  </si>
+  <si>
+    <t>10.1016/j.biopsycho.2018.02.018</t>
+  </si>
+  <si>
+    <t>Stress evokes stronger medial posterior cingulate deactivations during emotional distraction in slower paced aging</t>
+  </si>
+  <si>
+    <t>Oei, NYL; Jansen, SW; Veer, IM; Slagboom, PE; van de Grond, J; van Heemst, D</t>
+  </si>
+  <si>
+    <t>Introduction: Middle-aged offspring from long-lived families are thought to have a slower pace of aging, possibly related to HPA-axis function. Here, we investigated the neural and behavioral effects of social stress in offspring compared to their regular aging partners on emotional distraction during working memory (WM). Methods: 104 middle-aged participants (53 males) consisting of offspring and their partners underwent the Trier Social Stress Test or a control procedure. Hereafter, a WM task with emotional distracters was performed using fMRI. Saliva cortisol levels were obtained during the procedure. Results: Partners had higher overall cortisol levels than offspring. In addition, partners had decreased deactivations compared to offspring in the medial posterior cingulate cortex (mPCC) during emotional distraction, which were significantly correlated with lower accuracy during emotional distraction. Discussion: mPCC-deactivations are known to be modulated by chronological aging, with more deactivations in the young than in the old. Here we show the same pattern in familial longevity versus regular aging after mild stress, with more deactivations related to better accuracy during emotional distraction. Functional mPCC deactivations might thus be related to pace of aging, and can be revealed by inducing mild stress.</t>
   </si>
 </sst>
 </file>
@@ -852,7 +852,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1038,6 +1038,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -1208,11 +1214,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1571,12 +1578,13 @@
   <dimension ref="A1:N56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="A31" sqref="A31:XFD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="32.42578125" customWidth="1"/>
+    <col min="1" max="1" width="32.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
     <col min="7" max="7" width="15.140625" customWidth="1"/>
     <col min="8" max="8" width="18.5703125" customWidth="1"/>
     <col min="9" max="9" width="13.5703125" customWidth="1"/>
@@ -1592,7 +1600,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -1628,7 +1636,7 @@
         <v>11</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -1636,7 +1644,7 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -1666,7 +1674,7 @@
         <v>6</v>
       </c>
       <c r="L2">
-        <v>2.1666666666666701</v>
+        <v>1.9696969696969699</v>
       </c>
       <c r="M2">
         <v>1.56266666666667</v>
@@ -1677,40 +1685,40 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>2018</v>
+        <v>2011</v>
       </c>
       <c r="I3">
-        <v>21</v>
-      </c>
-      <c r="J3">
-        <v>0.25</v>
+        <v>103</v>
+      </c>
+      <c r="J3" t="s">
+        <v>25</v>
       </c>
       <c r="K3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L3">
-        <v>2.1</v>
-      </c>
-      <c r="M3">
-        <v>0.05</v>
+        <v>1.7166666666666699</v>
+      </c>
+      <c r="M3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -1718,40 +1726,40 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
       <c r="H4">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="I4">
-        <v>103</v>
-      </c>
-      <c r="J4" t="s">
-        <v>25</v>
+        <v>207</v>
+      </c>
+      <c r="J4">
+        <v>3.35</v>
       </c>
       <c r="K4">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="L4">
-        <v>1.9074074074074101</v>
-      </c>
-      <c r="M4" t="s">
-        <v>25</v>
+        <v>1.4375</v>
+      </c>
+      <c r="M4">
+        <v>0.20937500000000001</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -1759,40 +1767,40 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F5" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H5">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="I5">
-        <v>207</v>
+        <v>84</v>
       </c>
       <c r="J5">
-        <v>3.35</v>
+        <v>3</v>
       </c>
       <c r="K5">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="L5">
-        <v>1.6171875</v>
+        <v>1.4</v>
       </c>
       <c r="M5">
-        <v>0.20937500000000001</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1800,40 +1808,40 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H6">
-        <v>2009</v>
+        <v>2018</v>
       </c>
       <c r="I6">
-        <v>84</v>
+        <v>21</v>
       </c>
       <c r="J6">
-        <v>3</v>
+        <v>0.25</v>
       </c>
       <c r="K6">
         <v>5</v>
       </c>
       <c r="L6">
-        <v>1.52727272727273</v>
+        <v>1.4</v>
       </c>
       <c r="M6">
-        <v>0.6</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -1841,7 +1849,7 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="C7" t="s">
         <v>34</v>
@@ -1859,22 +1867,22 @@
         <v>1</v>
       </c>
       <c r="H7">
-        <v>2018</v>
+        <v>2009</v>
       </c>
       <c r="I7">
-        <v>3</v>
-      </c>
-      <c r="J7">
-        <v>4.0999999999999996</v>
+        <v>487</v>
+      </c>
+      <c r="J7" t="s">
+        <v>25</v>
       </c>
       <c r="K7">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="L7">
-        <v>1.5</v>
-      </c>
-      <c r="M7">
-        <v>4.0999999999999996</v>
+        <v>1.3527777777777801</v>
+      </c>
+      <c r="M7" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -1882,7 +1890,7 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="C8" t="s">
         <v>38</v>
@@ -1900,63 +1908,63 @@
         <v>1</v>
       </c>
       <c r="H8">
-        <v>2009</v>
+        <v>2013</v>
       </c>
       <c r="I8">
-        <v>487</v>
-      </c>
-      <c r="J8" t="s">
-        <v>25</v>
+        <v>97</v>
+      </c>
+      <c r="J8">
+        <v>212.91200000000001</v>
       </c>
       <c r="K8">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="L8">
-        <v>1.47575757575758</v>
-      </c>
-      <c r="M8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+        <v>1.2124999999999999</v>
+      </c>
+      <c r="M8">
+        <v>21.2912</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B9" t="s">
-        <v>194</v>
-      </c>
-      <c r="C9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" t="s">
-        <v>45</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9">
-        <v>2013</v>
-      </c>
-      <c r="I9">
-        <v>97</v>
-      </c>
-      <c r="J9">
-        <v>212.91200000000001</v>
-      </c>
-      <c r="K9">
-        <v>10</v>
-      </c>
-      <c r="L9">
-        <v>1.3857142857142899</v>
-      </c>
-      <c r="M9">
-        <v>21.2912</v>
+      <c r="B9" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="G9" s="4">
+        <v>1</v>
+      </c>
+      <c r="H9" s="4">
+        <v>2010</v>
+      </c>
+      <c r="I9" s="4">
+        <v>235</v>
+      </c>
+      <c r="J9" s="4">
+        <v>3</v>
+      </c>
+      <c r="K9" s="4">
+        <v>18</v>
+      </c>
+      <c r="L9" s="4">
+        <v>1.18686868686869</v>
+      </c>
+      <c r="M9" s="4">
+        <v>0.16666666666666699</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -1964,81 +1972,81 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E10" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F10" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H10">
-        <v>2016</v>
+        <v>2012</v>
       </c>
       <c r="I10">
-        <v>54</v>
+        <v>180</v>
       </c>
       <c r="J10">
-        <v>23.35</v>
+        <v>1195.48</v>
       </c>
       <c r="K10">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="L10">
-        <v>1.35</v>
+        <v>1.1764705882352899</v>
       </c>
       <c r="M10">
-        <v>2.335</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+        <v>70.322352941176504</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B11" t="s">
-        <v>196</v>
-      </c>
-      <c r="C11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" t="s">
-        <v>52</v>
-      </c>
-      <c r="F11" t="s">
-        <v>53</v>
-      </c>
-      <c r="G11">
-        <v>4</v>
-      </c>
-      <c r="H11">
-        <v>2012</v>
-      </c>
-      <c r="I11">
-        <v>180</v>
-      </c>
-      <c r="J11">
-        <v>1195.48</v>
-      </c>
-      <c r="K11">
-        <v>17</v>
-      </c>
-      <c r="L11">
-        <v>1.3235294117647101</v>
-      </c>
-      <c r="M11">
-        <v>70.322352941176504</v>
+      <c r="B11" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="G11" s="4">
+        <v>1</v>
+      </c>
+      <c r="H11" s="4">
+        <v>2009</v>
+      </c>
+      <c r="I11" s="4">
+        <v>268</v>
+      </c>
+      <c r="J11" s="4">
+        <v>195.35</v>
+      </c>
+      <c r="K11" s="4">
+        <v>19</v>
+      </c>
+      <c r="L11" s="4">
+        <v>1.1754385964912299</v>
+      </c>
+      <c r="M11" s="4">
+        <v>10.2815789473684</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -2059,22 +2067,22 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B13" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="E13" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="F13" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -2100,22 +2108,22 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B14" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="E14" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="F14" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="G14">
         <v>2</v>
@@ -2141,22 +2149,22 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" t="s">
+        <v>184</v>
+      </c>
+      <c r="C15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" t="s">
         <v>54</v>
-      </c>
-      <c r="B15" t="s">
-        <v>198</v>
-      </c>
-      <c r="C15" t="s">
-        <v>59</v>
-      </c>
-      <c r="D15" t="s">
-        <v>60</v>
-      </c>
-      <c r="E15" t="s">
-        <v>61</v>
-      </c>
-      <c r="F15" t="s">
-        <v>62</v>
       </c>
       <c r="G15">
         <v>1</v>
@@ -2182,22 +2190,22 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B16" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D16" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="E16" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="F16" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -2223,22 +2231,22 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B17" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="C17" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D17" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="E17" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="F17" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -2264,22 +2272,22 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B18" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="C18" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="D18" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E18" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="F18" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -2305,22 +2313,22 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B19" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="C19" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D19" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="E19" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="F19" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="G19">
         <v>2</v>
@@ -2346,22 +2354,22 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B20" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="C20" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D20" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="E20" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="F20" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -2387,22 +2395,22 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B21" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="C21" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D21" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="E21" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="F21" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -2428,22 +2436,22 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B22" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="C22" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D22" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E22" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F22" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -2485,22 +2493,22 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B24" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="C24" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D24" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="E24" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="F24" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="G24">
         <v>1</v>
@@ -2518,7 +2526,7 @@
         <v>1235</v>
       </c>
       <c r="L24">
-        <v>8.0971659919028304E-4</v>
+        <v>5.3981106612685601E-4</v>
       </c>
       <c r="M24">
         <v>3.5222672064777298E-3</v>
@@ -2526,22 +2534,22 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>79</v>
+      </c>
+      <c r="B25" t="s">
+        <v>192</v>
+      </c>
+      <c r="C25" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" t="s">
+        <v>85</v>
+      </c>
+      <c r="E25" t="s">
+        <v>86</v>
+      </c>
+      <c r="F25" t="s">
         <v>87</v>
-      </c>
-      <c r="B25" t="s">
-        <v>206</v>
-      </c>
-      <c r="C25" t="s">
-        <v>92</v>
-      </c>
-      <c r="D25" t="s">
-        <v>93</v>
-      </c>
-      <c r="E25" t="s">
-        <v>94</v>
-      </c>
-      <c r="F25" t="s">
-        <v>95</v>
       </c>
       <c r="G25">
         <v>1</v>
@@ -2559,7 +2567,7 @@
         <v>1263</v>
       </c>
       <c r="L25">
-        <v>1.18764845605701E-3</v>
+        <v>7.9176563737133805E-4</v>
       </c>
       <c r="M25">
         <v>7.9176563737133805E-4</v>
@@ -2567,22 +2575,22 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B26" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="C26" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D26" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="E26" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="F26" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="G26">
         <v>1</v>
@@ -2600,7 +2608,7 @@
         <v>1553</v>
       </c>
       <c r="L26">
-        <v>1.28783000643915E-3</v>
+        <v>9.6587250482936299E-4</v>
       </c>
       <c r="M26">
         <v>3.1229877656149402E-3</v>
@@ -2608,104 +2616,104 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B27" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="C27" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D27" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E27" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F27" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G27">
         <v>1</v>
       </c>
       <c r="H27">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="I27">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J27">
-        <v>0.75</v>
+        <v>76.900000000000006</v>
       </c>
       <c r="K27">
-        <v>320</v>
+        <v>165</v>
       </c>
       <c r="L27">
-        <v>2.5000000000000001E-3</v>
+        <v>2.0202020202020202E-3</v>
       </c>
       <c r="M27">
-        <v>2.3437499999999999E-3</v>
+        <v>0.46606060606060601</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B28" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="C28" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="D28" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="E28" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="F28" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="G28">
         <v>1</v>
       </c>
       <c r="H28">
-        <v>2018</v>
+        <v>2015</v>
       </c>
       <c r="I28">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J28">
-        <v>76.900000000000006</v>
+        <v>0.75</v>
       </c>
       <c r="K28">
-        <v>165</v>
+        <v>320</v>
       </c>
       <c r="L28">
-        <v>3.0303030303030299E-3</v>
+        <v>2.0833333333333298E-3</v>
       </c>
       <c r="M28">
-        <v>0.46606060606060601</v>
+        <v>2.3437499999999999E-3</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B29" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="C29" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D29" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E29" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="F29" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="G29">
         <v>1</v>
@@ -2723,7 +2731,7 @@
         <v>608</v>
       </c>
       <c r="L29">
-        <v>3.28947368421053E-3</v>
+        <v>2.6315789473684201E-3</v>
       </c>
       <c r="M29" t="s">
         <v>25</v>
@@ -2731,22 +2739,22 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B30" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="C30" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D30" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="E30" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="F30" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="G30">
         <v>1</v>
@@ -2764,71 +2772,71 @@
         <v>50</v>
       </c>
       <c r="L30">
-        <v>3.3333333333333301E-3</v>
+        <v>2.8571428571428602E-3</v>
       </c>
       <c r="M30">
         <v>0.03</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>87</v>
-      </c>
-      <c r="B31" t="s">
-        <v>212</v>
-      </c>
-      <c r="C31" t="s">
-        <v>116</v>
-      </c>
-      <c r="D31" t="s">
-        <v>117</v>
-      </c>
-      <c r="E31" t="s">
-        <v>118</v>
-      </c>
-      <c r="F31" t="s">
-        <v>119</v>
-      </c>
-      <c r="G31">
-        <v>1</v>
-      </c>
-      <c r="H31">
-        <v>2012</v>
-      </c>
-      <c r="I31">
-        <v>2</v>
-      </c>
-      <c r="J31">
-        <v>1.85</v>
-      </c>
-      <c r="K31">
-        <v>59</v>
-      </c>
-      <c r="L31">
-        <v>4.2372881355932203E-3</v>
-      </c>
-      <c r="M31">
-        <v>3.1355932203389801E-2</v>
+    <row r="31" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="G31" s="4">
+        <v>1</v>
+      </c>
+      <c r="H31" s="4">
+        <v>2018</v>
+      </c>
+      <c r="I31" s="4">
+        <v>1</v>
+      </c>
+      <c r="J31" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="K31" s="4">
+        <v>104</v>
+      </c>
+      <c r="L31" s="4">
+        <v>3.2051282051282098E-3</v>
+      </c>
+      <c r="M31" s="4">
+        <v>1.5384615384615399E-2</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B32" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="C32" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="D32" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="E32" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="F32" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="G32">
         <v>2</v>
@@ -2846,7 +2854,7 @@
         <v>306</v>
       </c>
       <c r="L32">
-        <v>4.3572984749455299E-3</v>
+        <v>3.26797385620915E-3</v>
       </c>
       <c r="M32">
         <v>4.65686274509804E-2</v>
@@ -2854,22 +2862,22 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B33" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="C33" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="D33" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="E33" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="F33" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="G33">
         <v>1</v>
@@ -2887,7 +2895,7 @@
         <v>76</v>
       </c>
       <c r="L33">
-        <v>4.3859649122806998E-3</v>
+        <v>3.28947368421053E-3</v>
       </c>
       <c r="M33">
         <v>2.1052631578947399E-2</v>
@@ -2927,22 +2935,22 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="B36" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="C36" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D36" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E36" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="F36" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="G36">
         <v>4</v>
@@ -2960,7 +2968,7 @@
         <v>17</v>
       </c>
       <c r="L36">
-        <v>1.3235294117647101</v>
+        <v>1.1764705882352899</v>
       </c>
       <c r="M36">
         <v>70.322352941176504</v>
@@ -2968,22 +2976,22 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="B37" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="C37" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="D37" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="E37" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="F37" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="G37">
         <v>1</v>
@@ -3001,7 +3009,7 @@
         <v>11</v>
       </c>
       <c r="L37">
-        <v>0.83838383838383801</v>
+        <v>0.75454545454545496</v>
       </c>
       <c r="M37">
         <v>57.185272727272697</v>
@@ -3009,22 +3017,22 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="B38" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="C38" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="D38" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="E38" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="F38" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="G38">
         <v>1</v>
@@ -3042,7 +3050,7 @@
         <v>24</v>
       </c>
       <c r="L38">
-        <v>0.65277777777777801</v>
+        <v>0.48958333333333298</v>
       </c>
       <c r="M38">
         <v>48.656500000000001</v>
@@ -3050,22 +3058,22 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>116</v>
+      </c>
+      <c r="B39" t="s">
+        <v>202</v>
+      </c>
+      <c r="C39" t="s">
+        <v>125</v>
+      </c>
+      <c r="D39" t="s">
+        <v>126</v>
+      </c>
+      <c r="E39" t="s">
+        <v>127</v>
+      </c>
+      <c r="F39" t="s">
         <v>128</v>
-      </c>
-      <c r="B39" t="s">
-        <v>217</v>
-      </c>
-      <c r="C39" t="s">
-        <v>137</v>
-      </c>
-      <c r="D39" t="s">
-        <v>138</v>
-      </c>
-      <c r="E39" t="s">
-        <v>139</v>
-      </c>
-      <c r="F39" t="s">
-        <v>140</v>
       </c>
       <c r="G39">
         <v>2</v>
@@ -3083,7 +3091,7 @@
         <v>25</v>
       </c>
       <c r="L39">
-        <v>0.96</v>
+        <v>0.87272727272727302</v>
       </c>
       <c r="M39">
         <v>45.727519999999998</v>
@@ -3091,22 +3099,22 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="B40" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="C40" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="D40" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="E40" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="F40" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="G40">
         <v>1</v>
@@ -3124,7 +3132,7 @@
         <v>18</v>
       </c>
       <c r="L40">
-        <v>0.59876543209876498</v>
+        <v>0.53888888888888897</v>
       </c>
       <c r="M40">
         <v>30.814444444444401</v>
@@ -3132,22 +3140,22 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="B41" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="C41" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="D41" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="E41" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="F41" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="G41">
         <v>3</v>
@@ -3165,7 +3173,7 @@
         <v>14</v>
       </c>
       <c r="L41">
-        <v>3.5714285714285698E-2</v>
+        <v>2.3809523809523801E-2</v>
       </c>
       <c r="M41">
         <v>26.62</v>
@@ -3173,22 +3181,22 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="B42" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="C42" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D42" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="E42" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="F42" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="G42">
         <v>1</v>
@@ -3206,7 +3214,7 @@
         <v>40</v>
       </c>
       <c r="L42">
-        <v>0.75833333333333297</v>
+        <v>0.6825</v>
       </c>
       <c r="M42">
         <v>22.070049999999998</v>
@@ -3214,22 +3222,22 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="B43" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="C43" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="D43" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="E43" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="F43" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="G43">
         <v>1</v>
@@ -3247,7 +3255,7 @@
         <v>12</v>
       </c>
       <c r="L43">
-        <v>0.42857142857142899</v>
+        <v>0.375</v>
       </c>
       <c r="M43">
         <v>22.037500000000001</v>
@@ -3255,22 +3263,22 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="B44" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="C44" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D44" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E44" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F44" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G44">
         <v>1</v>
@@ -3288,7 +3296,7 @@
         <v>10</v>
       </c>
       <c r="L44">
-        <v>1.3857142857142899</v>
+        <v>1.2124999999999999</v>
       </c>
       <c r="M44">
         <v>21.2912</v>
@@ -3296,22 +3304,22 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="B45" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="C45" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="D45" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="E45" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="F45" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="G45">
         <v>1</v>
@@ -3329,7 +3337,7 @@
         <v>18</v>
       </c>
       <c r="L45">
-        <v>0.52777777777777801</v>
+        <v>0.452380952380952</v>
       </c>
       <c r="M45">
         <v>19.956333333333301</v>
@@ -3353,22 +3361,22 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="B47" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="C47" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D47" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E47" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="F47" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="G47">
         <v>1</v>
@@ -3386,7 +3394,7 @@
         <v>1263</v>
       </c>
       <c r="L47">
-        <v>1.18764845605701E-3</v>
+        <v>7.9176563737133805E-4</v>
       </c>
       <c r="M47">
         <v>7.9176563737133805E-4</v>
@@ -3394,22 +3402,22 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="B48" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="C48" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="D48" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="E48" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="F48" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="G48">
         <v>1</v>
@@ -3427,7 +3435,7 @@
         <v>298</v>
       </c>
       <c r="L48">
-        <v>5.0335570469798698E-3</v>
+        <v>4.0268456375838896E-3</v>
       </c>
       <c r="M48">
         <v>8.3892617449664395E-4</v>
@@ -3435,22 +3443,22 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="B49" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="C49" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="D49" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="E49" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="F49" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="G49">
         <v>1</v>
@@ -3468,7 +3476,7 @@
         <v>291</v>
       </c>
       <c r="L49">
-        <v>1.03092783505155E-2</v>
+        <v>8.2474226804123696E-3</v>
       </c>
       <c r="M49">
         <v>8.5910652920962198E-4</v>
@@ -3476,22 +3484,22 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>149</v>
+      </c>
+      <c r="B50" t="s">
+        <v>210</v>
+      </c>
+      <c r="C50" t="s">
+        <v>158</v>
+      </c>
+      <c r="D50" t="s">
+        <v>159</v>
+      </c>
+      <c r="E50" t="s">
+        <v>160</v>
+      </c>
+      <c r="F50" t="s">
         <v>161</v>
-      </c>
-      <c r="B50" t="s">
-        <v>225</v>
-      </c>
-      <c r="C50" t="s">
-        <v>170</v>
-      </c>
-      <c r="D50" t="s">
-        <v>171</v>
-      </c>
-      <c r="E50" t="s">
-        <v>172</v>
-      </c>
-      <c r="F50" t="s">
-        <v>173</v>
       </c>
       <c r="G50">
         <v>1</v>
@@ -3509,7 +3517,7 @@
         <v>1277</v>
       </c>
       <c r="L50">
-        <v>6.5257113025319804E-3</v>
+        <v>4.8942834768989796E-3</v>
       </c>
       <c r="M50">
         <v>1.1746280344557599E-3</v>
@@ -3517,22 +3525,22 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="B51" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="C51" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="D51" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="E51" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="F51" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="G51">
         <v>1</v>
@@ -3550,7 +3558,7 @@
         <v>264</v>
       </c>
       <c r="L51">
-        <v>1.0416666666666701E-2</v>
+        <v>8.3333333333333297E-3</v>
       </c>
       <c r="M51">
         <v>1.8939393939393901E-3</v>
@@ -3558,22 +3566,22 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="B52" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="C52" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D52" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="E52" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="F52" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="G52">
         <v>1</v>
@@ -3591,7 +3599,7 @@
         <v>320</v>
       </c>
       <c r="L52">
-        <v>2.5000000000000001E-3</v>
+        <v>2.0833333333333298E-3</v>
       </c>
       <c r="M52">
         <v>2.3437499999999999E-3</v>
@@ -3599,22 +3607,22 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="B53" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="C53" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="D53" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="E53" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="F53" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="G53">
         <v>1</v>
@@ -3632,7 +3640,7 @@
         <v>85</v>
       </c>
       <c r="L53">
-        <v>1.7647058823529401E-2</v>
+        <v>1.1764705882352899E-2</v>
       </c>
       <c r="M53">
         <v>2.94117647058824E-3</v>
@@ -3640,22 +3648,22 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="B54" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
       <c r="C54" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="D54" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="E54" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="F54" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="G54">
         <v>1</v>
@@ -3673,7 +3681,7 @@
         <v>561</v>
       </c>
       <c r="L54">
-        <v>8.4670231729055308E-3</v>
+        <v>6.7736185383244201E-3</v>
       </c>
       <c r="M54">
         <v>3.1194295900178301E-3</v>
@@ -3681,22 +3689,22 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="B55" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="C55" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D55" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="E55" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="F55" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="G55">
         <v>1</v>
@@ -3714,7 +3722,7 @@
         <v>1553</v>
       </c>
       <c r="L55">
-        <v>1.28783000643915E-3</v>
+        <v>9.6587250482936299E-4</v>
       </c>
       <c r="M55">
         <v>3.1229877656149402E-3</v>
@@ -3722,22 +3730,22 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="B56" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="C56" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D56" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="E56" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="F56" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="G56">
         <v>1</v>
@@ -3755,7 +3763,7 @@
         <v>1235</v>
       </c>
       <c r="L56">
-        <v>8.0971659919028304E-4</v>
+        <v>5.3981106612685601E-4</v>
       </c>
       <c r="M56">
         <v>3.5222672064777298E-3</v>

</xml_diff>